<commit_message>
Waffle Chart As Pie Chart Replacement
</commit_message>
<xml_diff>
--- a/WaffleChart.xlsx
+++ b/WaffleChart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{4DDFA2C6-FAD9-4AD3-AD50-498E7BB6B6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71C2A987-A859-4BCA-B0E5-B1264A3E970E}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{4DDFA2C6-FAD9-4AD3-AD50-498E7BB6B6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C41984B8-5ABF-4D0A-9FE9-FD7DD2DCAB60}"/>
   <bookViews>
-    <workbookView xWindow="2475" yWindow="1980" windowWidth="21600" windowHeight="11385" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="4620" yWindow="855" windowWidth="21600" windowHeight="11385" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Waffle" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>FROM:</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>Can I use a waffle chart like a pie chart?</t>
   </si>
 </sst>
 </file>
@@ -168,7 +171,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,6 +199,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -271,12 +280,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -294,7 +304,59 @@
     <cellStyle name="Title" xfId="1" builtinId="15" hidden="1"/>
     <cellStyle name="Total" xfId="6" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="17">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -415,13 +477,13 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Biegert Table Standard" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Biegert Table Standard" pivot="0" count="7" xr9:uid="{95B43237-2845-4068-A415-A5A3E7804959}">
-      <tableStyleElement type="wholeTable" dxfId="9"/>
-      <tableStyleElement type="headerRow" dxfId="8"/>
-      <tableStyleElement type="totalRow" dxfId="7"/>
-      <tableStyleElement type="firstColumn" dxfId="6"/>
-      <tableStyleElement type="lastColumn" dxfId="5"/>
-      <tableStyleElement type="firstRowStripe" dxfId="4"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="3"/>
+      <tableStyleElement type="wholeTable" dxfId="16"/>
+      <tableStyleElement type="headerRow" dxfId="15"/>
+      <tableStyleElement type="totalRow" dxfId="14"/>
+      <tableStyleElement type="firstColumn" dxfId="13"/>
+      <tableStyleElement type="lastColumn" dxfId="12"/>
+      <tableStyleElement type="firstRowStripe" dxfId="11"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="10"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -440,13 +502,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -463,7 +525,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="628650" y="1133475"/>
+          <a:off x="609600" y="1133475"/>
           <a:ext cx="3790950" cy="1619250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -545,7 +607,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$B$8:$K$17" spid="_x0000_s1030"/>
+                  <a14:cameraTool cellRange="$B$8:$K$17" spid="_x0000_s1032"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -773,10 +835,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB114D2F-F620-446A-92CE-0CB3C9FD0F74}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1108,7 +1170,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B17" s="3">
         <v>1</v>
       </c>
@@ -1140,13 +1202,355 @@
         <v>10</v>
       </c>
     </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L20">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="L21">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B24" s="5" cm="1">
+        <f t="array" ref="B24:K33">_xlfn._xlws.SORT(_xlfn.SEQUENCE(10,10),,-1)</f>
+        <v>91</v>
+      </c>
+      <c r="C24" s="5">
+        <v>92</v>
+      </c>
+      <c r="D24" s="5">
+        <v>93</v>
+      </c>
+      <c r="E24" s="5">
+        <v>94</v>
+      </c>
+      <c r="F24" s="5">
+        <v>95</v>
+      </c>
+      <c r="G24" s="5">
+        <v>96</v>
+      </c>
+      <c r="H24" s="5">
+        <v>97</v>
+      </c>
+      <c r="I24" s="5">
+        <v>98</v>
+      </c>
+      <c r="J24" s="5">
+        <v>99</v>
+      </c>
+      <c r="K24" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B25" s="5">
+        <v>81</v>
+      </c>
+      <c r="C25" s="5">
+        <v>82</v>
+      </c>
+      <c r="D25" s="5">
+        <v>83</v>
+      </c>
+      <c r="E25" s="5">
+        <v>84</v>
+      </c>
+      <c r="F25" s="5">
+        <v>85</v>
+      </c>
+      <c r="G25" s="5">
+        <v>86</v>
+      </c>
+      <c r="H25" s="5">
+        <v>87</v>
+      </c>
+      <c r="I25" s="5">
+        <v>88</v>
+      </c>
+      <c r="J25" s="5">
+        <v>89</v>
+      </c>
+      <c r="K25" s="5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B26" s="5">
+        <v>71</v>
+      </c>
+      <c r="C26" s="5">
+        <v>72</v>
+      </c>
+      <c r="D26" s="5">
+        <v>73</v>
+      </c>
+      <c r="E26" s="5">
+        <v>74</v>
+      </c>
+      <c r="F26" s="5">
+        <v>75</v>
+      </c>
+      <c r="G26" s="5">
+        <v>76</v>
+      </c>
+      <c r="H26" s="5">
+        <v>77</v>
+      </c>
+      <c r="I26" s="5">
+        <v>78</v>
+      </c>
+      <c r="J26" s="5">
+        <v>79</v>
+      </c>
+      <c r="K26" s="5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B27" s="5">
+        <v>61</v>
+      </c>
+      <c r="C27" s="5">
+        <v>62</v>
+      </c>
+      <c r="D27" s="5">
+        <v>63</v>
+      </c>
+      <c r="E27" s="5">
+        <v>64</v>
+      </c>
+      <c r="F27" s="5">
+        <v>65</v>
+      </c>
+      <c r="G27" s="5">
+        <v>66</v>
+      </c>
+      <c r="H27" s="5">
+        <v>67</v>
+      </c>
+      <c r="I27" s="5">
+        <v>68</v>
+      </c>
+      <c r="J27" s="5">
+        <v>69</v>
+      </c>
+      <c r="K27" s="5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B28" s="5">
+        <v>51</v>
+      </c>
+      <c r="C28" s="5">
+        <v>52</v>
+      </c>
+      <c r="D28" s="5">
+        <v>53</v>
+      </c>
+      <c r="E28" s="5">
+        <v>54</v>
+      </c>
+      <c r="F28" s="5">
+        <v>55</v>
+      </c>
+      <c r="G28" s="5">
+        <v>56</v>
+      </c>
+      <c r="H28" s="5">
+        <v>57</v>
+      </c>
+      <c r="I28" s="5">
+        <v>58</v>
+      </c>
+      <c r="J28" s="5">
+        <v>59</v>
+      </c>
+      <c r="K28" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B29" s="5">
+        <v>41</v>
+      </c>
+      <c r="C29" s="5">
+        <v>42</v>
+      </c>
+      <c r="D29" s="5">
+        <v>43</v>
+      </c>
+      <c r="E29" s="5">
+        <v>44</v>
+      </c>
+      <c r="F29" s="5">
+        <v>45</v>
+      </c>
+      <c r="G29" s="5">
+        <v>46</v>
+      </c>
+      <c r="H29" s="5">
+        <v>47</v>
+      </c>
+      <c r="I29" s="5">
+        <v>48</v>
+      </c>
+      <c r="J29" s="5">
+        <v>49</v>
+      </c>
+      <c r="K29" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B30" s="5">
+        <v>31</v>
+      </c>
+      <c r="C30" s="5">
+        <v>32</v>
+      </c>
+      <c r="D30" s="5">
+        <v>33</v>
+      </c>
+      <c r="E30" s="5">
+        <v>34</v>
+      </c>
+      <c r="F30" s="5">
+        <v>35</v>
+      </c>
+      <c r="G30" s="5">
+        <v>36</v>
+      </c>
+      <c r="H30" s="5">
+        <v>37</v>
+      </c>
+      <c r="I30" s="5">
+        <v>38</v>
+      </c>
+      <c r="J30" s="5">
+        <v>39</v>
+      </c>
+      <c r="K30" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B31" s="5">
+        <v>21</v>
+      </c>
+      <c r="C31" s="5">
+        <v>22</v>
+      </c>
+      <c r="D31" s="5">
+        <v>23</v>
+      </c>
+      <c r="E31" s="5">
+        <v>24</v>
+      </c>
+      <c r="F31" s="5">
+        <v>25</v>
+      </c>
+      <c r="G31" s="5">
+        <v>26</v>
+      </c>
+      <c r="H31" s="5">
+        <v>27</v>
+      </c>
+      <c r="I31" s="5">
+        <v>28</v>
+      </c>
+      <c r="J31" s="5">
+        <v>29</v>
+      </c>
+      <c r="K31" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B32" s="5">
+        <v>11</v>
+      </c>
+      <c r="C32" s="5">
+        <v>12</v>
+      </c>
+      <c r="D32" s="5">
+        <v>13</v>
+      </c>
+      <c r="E32" s="5">
+        <v>14</v>
+      </c>
+      <c r="F32" s="5">
+        <v>15</v>
+      </c>
+      <c r="G32" s="5">
+        <v>16</v>
+      </c>
+      <c r="H32" s="5">
+        <v>17</v>
+      </c>
+      <c r="I32" s="5">
+        <v>18</v>
+      </c>
+      <c r="J32" s="5">
+        <v>19</v>
+      </c>
+      <c r="K32" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B33" s="5">
+        <v>1</v>
+      </c>
+      <c r="C33" s="5">
+        <v>2</v>
+      </c>
+      <c r="D33" s="5">
+        <v>3</v>
+      </c>
+      <c r="E33" s="5">
+        <v>4</v>
+      </c>
+      <c r="F33" s="5">
+        <v>5</v>
+      </c>
+      <c r="G33" s="5">
+        <v>6</v>
+      </c>
+      <c r="H33" s="5">
+        <v>7</v>
+      </c>
+      <c r="I33" s="5">
+        <v>8</v>
+      </c>
+      <c r="J33" s="5">
+        <v>9</v>
+      </c>
+      <c r="K33" s="5">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B8:K17">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="lessThan">
       <formula>$N$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="lessThanOrEqual">
       <formula>$N$2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24:K33">
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>B24&lt;=$L$20</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="2">
+      <formula>B24&lt;=$L$21+$L$20</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>